<commit_message>
Plan reMake 3DPlayer Bug
</commit_message>
<xml_diff>
--- a/ゲームプログラミング制作2年ver.1.8（3DMap制作開始）/企画書.xlsx
+++ b/ゲームプログラミング制作2年ver.1.8（3DMap制作開始）/企画書.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junichi\Desktop\ゲームプログラミング制作2年ver.1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junichi\Desktop\BLOCK-CRASH\BLOCK-CRASH\ゲームプログラミング制作2年ver.1.8（3DMap制作開始）\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2293A36D-4690-40B5-A547-F3CE5A19873B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10560"/>
+    <workbookView xWindow="9270" yWindow="1650" windowWidth="12615" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>1,概要</t>
     <rPh sb="2" eb="4">
@@ -33,28 +34,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>画面上に配置するブロックは自分で指定。（可能ならランダム）</t>
-    <rPh sb="0" eb="2">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ハイチ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>カノウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・マップの仕組み</t>
     <rPh sb="5" eb="7">
       <t>シク</t>
@@ -62,87 +41,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>プレイヤーを画面下部に配置</t>
-    <rPh sb="6" eb="8">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>カブ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ハイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ボードを操作してボールをはじき、ブロックを壊していくゲーム</t>
-    <rPh sb="4" eb="6">
-      <t>ソウサ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>コワ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ボールをプレイヤーの初期値の少し上（+15.0）に配置</t>
-    <rPh sb="10" eb="13">
-      <t>ショキチ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ハイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>画面両端に柱（移動制御用のため）を配置</t>
-    <rPh sb="0" eb="2">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>リョウハジ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ハシラ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ハイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>これに当たっても弾は反射する。</t>
-    <rPh sb="3" eb="4">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>タマ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ハンシャ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>回るブロックや動くブロックをギミックとして配置</t>
-    <rPh sb="0" eb="1">
-      <t>マワ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ウゴ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ハイチ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・プレイヤーの仕組み</t>
     <rPh sb="7" eb="9">
       <t>シク</t>
@@ -150,47 +48,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>プレイヤーは左右に移動可能（奥行き実装予定）</t>
-    <rPh sb="6" eb="8">
-      <t>サユウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>イドウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>カノウ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>オクユ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ジッソウ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ヨテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>左右に傾けることができ、ボールの反射方向を変えることができる</t>
-    <rPh sb="0" eb="2">
-      <t>サユウ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>カタム</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ハンシャ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ホウコウ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>カ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・ボールの仕組み</t>
     <rPh sb="5" eb="7">
       <t>シク</t>
@@ -198,15 +55,384 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>重力を持ちながら上下にバウンドする</t>
+    <t>回転する板を操作してボールをはじき、ブロックにボールを当ててスコアを稼ぐゲームゲーム</t>
     <rPh sb="0" eb="2">
-      <t>ジュウリョク</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>モ</t>
-    </rPh>
+      <t>カイテン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>イタ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>カセ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>大まかに自分が操作できる回転する板、跳ね返すボール、点数を稼ぐための様々なブロックがある。</t>
+    <rPh sb="0" eb="1">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイテン</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>イタ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ハ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>カエ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>テンスウ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>カセ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>サマザマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1wavw,ギミックを理解させて点数を稼ぐ。</t>
+    <rPh sb="11" eb="13">
+      <t>リカイ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>テンスウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カセ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2wavw,ギミックの応用。こんな使い方もできるのか、的なものを感じさせる</t>
+    <rPh sb="11" eb="13">
+      <t>オウヨウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>テキ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>カン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・ゲームの流れ</t>
+    <rPh sb="5" eb="6">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wave形式のステージでギミックや様々なブロックを生かして点数を稼いでいく。</t>
+    <rPh sb="4" eb="6">
+      <t>ケイシキ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>サマザマ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>テンスウ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>カセ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3wave終了でリザルトへ。合計点でランクが決められる。</t>
+    <rPh sb="5" eb="7">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ゴウケイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>テン</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3wave,ボスのようなブロックを置く。ギミックをうまく使い、大きい目的を達成させる。達成で得点大量ゲット</t>
+    <rPh sb="17" eb="18">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>タッセイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>タッセイ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>トクテン</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>タイリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HPが０になるとゲームオーバーとなる。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3D空間でのブロック崩し風ゲーム。</t>
+    <rPh sb="2" eb="4">
+      <t>クウカン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>クズ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>フウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ステージが全部で３つ。Easy,Normal,Difficult。</t>
+    <rPh sb="5" eb="7">
+      <t>ゼンブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1ステージに3つのWaveを用意。</t>
+    <rPh sb="14" eb="16">
+      <t>ヨウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>当たったブロックの面に応じて上下にバウンドする。</t>
+    <rPh sb="0" eb="1">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>メン</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>オウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ジョウゲ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>マウスの動きに連動して縦回転、横回転、奥回転するようになっている。</t>
+    <rPh sb="4" eb="5">
+      <t>ウゴ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>レンドウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>タテ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイテン</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ヨコ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カイテン</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>オク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カイテン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブロックに当たれば当たるほど速度が増していきどんどん難しくなっていく。</t>
+    <rPh sb="5" eb="6">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ソクド</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>マ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ムズカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>当たってはいけないブロックやアイテムに当たると最初にいた場所へリスポーンする。</t>
+    <rPh sb="0" eb="1">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>バショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>当たったものによってポイント加算や減算、HP減少など様々な効果が得られる。</t>
+    <rPh sb="0" eb="1">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>カサン</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゲンザン</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ゲンショウ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>サマザマ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>コウカ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>エ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2,操作方法</t>
+    <rPh sb="2" eb="4">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ホウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w,s…ステージ選択上下</t>
     <rPh sb="8" eb="10">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="10" eb="12">
       <t>ジョウゲ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Space…ボールの動き開始</t>
+    <rPh sb="10" eb="11">
+      <t>ウゴ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enter…ステージ決定</t>
+    <rPh sb="10" eb="12">
+      <t>ケッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3,面白ポイント</t>
+    <rPh sb="2" eb="4">
+      <t>オモシロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>早くなっていくボールを制御しつつ、高得点を稼ぐ、スピード感が楽しめる！</t>
+    <rPh sb="0" eb="1">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>セイギョ</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>コウトクテン</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>カセ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>タノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>様々なステージギミックがあり、いろんな攻略法がある、ワンパターンではない。</t>
+    <rPh sb="0" eb="2">
+      <t>サマザマ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>コウリャクホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新感覚！3D空間で、奥行きのあるブロック崩し！</t>
+    <rPh sb="0" eb="3">
+      <t>シンカンカク</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>クウカン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>オクユ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>クズ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -214,7 +440,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,9 +480,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,16 +766,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="60.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.4">
@@ -554,6 +783,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>4</v>
@@ -561,62 +795,132 @@
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B17" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>